<commit_message>
refactor: Script work + thumb support on gallery
</commit_message>
<xml_diff>
--- a/utilities/data/import.xlsx
+++ b/utilities/data/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\BraveSnouts\utilities\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B3AB2-2E78-4733-B8C9-C7E86A29E858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E36438-A886-4CFF-B50B-62F670E07C6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{53AA4BC8-B5CE-417A-A802-26D6AE29237A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>Ime</t>
   </si>
@@ -150,103 +150,16 @@
     <t>Test33</t>
   </si>
   <si>
-    <t>4.jpg</t>
-  </si>
-  <si>
-    <t>5.jpg</t>
-  </si>
-  <si>
-    <t>7.jpg</t>
-  </si>
-  <si>
-    <t>8.jpg</t>
-  </si>
-  <si>
-    <t>9.jpg</t>
-  </si>
-  <si>
-    <t>10.jpg</t>
-  </si>
-  <si>
-    <t>11.jpg</t>
-  </si>
-  <si>
-    <t>0.jpg</t>
-  </si>
-  <si>
-    <t>1.jpg</t>
-  </si>
-  <si>
-    <t>2.jpg</t>
-  </si>
-  <si>
-    <t>3.jpg</t>
-  </si>
-  <si>
-    <t>6.jpg</t>
-  </si>
-  <si>
-    <t>12.jpg</t>
-  </si>
-  <si>
-    <t>13.jpg</t>
-  </si>
-  <si>
-    <t>14.jpg</t>
-  </si>
-  <si>
-    <t>15.jpg</t>
-  </si>
-  <si>
-    <t>16.jpg</t>
-  </si>
-  <si>
-    <t>17.jpg</t>
-  </si>
-  <si>
-    <t>18.jpg</t>
-  </si>
-  <si>
-    <t>19.jpg</t>
-  </si>
-  <si>
-    <t>20.jpg</t>
-  </si>
-  <si>
-    <t>21.jpg</t>
-  </si>
-  <si>
-    <t>22.jpg</t>
-  </si>
-  <si>
-    <t>23.jpg</t>
-  </si>
-  <si>
-    <t>24.jpg</t>
-  </si>
-  <si>
-    <t>25.jpg</t>
-  </si>
-  <si>
-    <t>26.jpg</t>
-  </si>
-  <si>
-    <t>27.jpg</t>
-  </si>
-  <si>
-    <t>28.jpg</t>
-  </si>
-  <si>
-    <t>29.jpg</t>
-  </si>
-  <si>
-    <t>30.jpg</t>
-  </si>
-  <si>
-    <t>31.jpg</t>
-  </si>
-  <si>
-    <t>32.jpg</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>0, 34, 36</t>
+  </si>
+  <si>
+    <t>2, 48, 56</t>
+  </si>
+  <si>
+    <t>5, 85</t>
   </si>
 </sst>
 </file>
@@ -604,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E40FBAA-BB98-465F-AFC2-890F31591454}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,480 +528,579 @@
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
+      <c r="C9">
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
+      <c r="C20">
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
+      <c r="C21">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
+      <c r="C22">
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
+      <c r="C25">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3</v>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
+      <c r="C27">
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3</v>
+      <c r="C29">
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3</v>
+      <c r="C30">
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
+      <c r="C31">
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
+      <c r="C32">
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
+      <c r="C33">
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3</v>
+      <c r="C34">
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>